<commit_message>
Edit profile and spin flow
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/INP1.xlsx
+++ b/src/main/resources/dataSheets/INP1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssivaramakrishnan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9351764C-EB02-4BFA-8822-297897392F48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78799D8-BE43-42E5-9B65-35B8B8DEC724}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{617CFBA4-D7F4-45BB-869F-6F644B8E70CF}"/>
   </bookViews>
@@ -33,10 +33,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>fsqa2tpn@gmail.com</t>
+    <t>Admin@123</t>
   </si>
   <si>
-    <t>Admin@123</t>
+    <t>tpnqatest@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -420,10 +420,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>